<commit_message>
updated 3-2 at middark 30 [clown music]
</commit_message>
<xml_diff>
--- a/Admin/Ara Folder/Spring Semester/Timesheet_2-6_2-12.xlsx
+++ b/Admin/Ara Folder/Spring Semester/Timesheet_2-6_2-12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borde\Senior Design Project\Admin\Ara Folder\Spring Semester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD2B64-D691-4E8C-917F-DAD3BCC56B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80024AA8-D5CB-4B40-BF6F-3F39CB08ACED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1BC5497-AAD9-4DDC-8628-751A33E9D351}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,25 +622,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>44592</v>
+        <v>44598</v>
       </c>
       <c r="C5" s="4">
-        <v>44593</v>
+        <v>44599</v>
       </c>
       <c r="D5" s="4">
-        <v>44594</v>
+        <v>44600</v>
       </c>
       <c r="E5" s="4">
-        <v>44595</v>
+        <v>44601</v>
       </c>
       <c r="F5" s="4">
-        <v>44596</v>
+        <v>44602</v>
       </c>
       <c r="G5" s="4">
-        <v>44597</v>
+        <v>44603</v>
       </c>
       <c r="H5" s="5">
-        <v>44598</v>
+        <v>44604</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>6</v>
@@ -685,13 +685,15 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -701,13 +703,15 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8">
+        <v>1.5</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
       <c r="I9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -717,13 +721,15 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -824,7 +830,7 @@
       </c>
       <c r="E16" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="1"/>
@@ -840,7 +846,7 @@
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>